<commit_message>
New excel logic New job, old job, P, L, DB columns
</commit_message>
<xml_diff>
--- a/protocol/Custom.xlsx
+++ b/protocol/Custom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Apollo files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52303C3D-EB5A-42F6-A6D6-B67BC942C4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A4B3BE-61A6-43CC-9DCB-918D4928179C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="50">
   <si>
     <t>Tests</t>
   </si>
@@ -155,18 +155,6 @@
     <t>Foot Print Data</t>
   </si>
   <si>
-    <t>IPref</t>
-  </si>
-  <si>
-    <t>0.8·IPref</t>
-  </si>
-  <si>
-    <t>1.0·IPref</t>
-  </si>
-  <si>
-    <t>1.2·IPref</t>
-  </si>
-  <si>
     <t>L5</t>
   </si>
   <si>
@@ -177,6 +165,18 @@
   </si>
   <si>
     <t>+/-3</t>
+  </si>
+  <si>
+    <t>Job</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Old Job</t>
   </si>
 </sst>
 </file>
@@ -222,7 +222,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -613,11 +613,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58031019-AFD2-4461-8B24-C325E2174DEC}">
-  <dimension ref="A1:K90"/>
+  <dimension ref="A1:M90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <pane ySplit="2" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -635,7 +635,7 @@
     <col min="15" max="15" width="22.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="25.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="25.8" x14ac:dyDescent="0.3">
       <c r="B1" s="12" t="s">
         <v>21</v>
       </c>
@@ -646,8 +646,12 @@
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
-    </row>
-    <row r="2" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+    </row>
+    <row r="2" spans="1:13" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -679,10 +683,16 @@
         <v>40</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>23</v>
       </c>
@@ -716,8 +726,14 @@
       <c r="K3" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>23</v>
       </c>
@@ -751,8 +767,14 @@
       <c r="K4" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>23</v>
       </c>
@@ -786,8 +808,14 @@
       <c r="K5" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>23</v>
       </c>
@@ -821,8 +849,14 @@
       <c r="K6" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>23</v>
       </c>
@@ -856,8 +890,14 @@
       <c r="K7" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>23</v>
       </c>
@@ -891,8 +931,14 @@
       <c r="K8" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>23</v>
       </c>
@@ -926,8 +972,14 @@
       <c r="K9" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>23</v>
       </c>
@@ -961,8 +1013,14 @@
       <c r="K10" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>23</v>
       </c>
@@ -996,8 +1054,14 @@
       <c r="K11" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>23</v>
       </c>
@@ -1031,8 +1095,14 @@
       <c r="K12" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>23</v>
       </c>
@@ -1066,8 +1136,14 @@
       <c r="K13" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>23</v>
       </c>
@@ -1101,8 +1177,14 @@
       <c r="K14" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>23</v>
       </c>
@@ -1136,8 +1218,14 @@
       <c r="K15" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>23</v>
       </c>
@@ -1171,8 +1259,14 @@
       <c r="K16" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>23</v>
       </c>
@@ -1206,8 +1300,14 @@
       <c r="K17" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>23</v>
       </c>
@@ -1241,8 +1341,14 @@
       <c r="K18" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>23</v>
       </c>
@@ -1276,8 +1382,14 @@
       <c r="K19" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>23</v>
       </c>
@@ -1311,8 +1423,14 @@
       <c r="K20" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>23</v>
       </c>
@@ -1346,8 +1464,14 @@
       <c r="K21" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>23</v>
       </c>
@@ -1381,8 +1505,14 @@
       <c r="K22" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>23</v>
       </c>
@@ -1416,8 +1546,14 @@
       <c r="K23" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>23</v>
       </c>
@@ -1451,8 +1587,14 @@
       <c r="K24" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>23</v>
       </c>
@@ -1486,8 +1628,14 @@
       <c r="K25" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>23</v>
       </c>
@@ -1521,8 +1669,14 @@
       <c r="K26" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>23</v>
       </c>
@@ -1556,8 +1710,14 @@
       <c r="K27" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>23</v>
       </c>
@@ -1591,8 +1751,14 @@
       <c r="K28" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>23</v>
       </c>
@@ -1626,8 +1792,14 @@
       <c r="K29" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>23</v>
       </c>
@@ -1661,8 +1833,14 @@
       <c r="K30" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>23</v>
       </c>
@@ -1696,8 +1874,14 @@
       <c r="K31" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>23</v>
       </c>
@@ -1731,8 +1915,14 @@
       <c r="K32" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>24</v>
       </c>
@@ -1766,8 +1956,14 @@
       <c r="K33" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>24</v>
       </c>
@@ -1801,8 +1997,14 @@
       <c r="K34" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>24</v>
       </c>
@@ -1836,8 +2038,14 @@
       <c r="K35" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L35" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>24</v>
       </c>
@@ -1871,8 +2079,14 @@
       <c r="K36" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>24</v>
       </c>
@@ -1906,8 +2120,14 @@
       <c r="K37" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>24</v>
       </c>
@@ -1941,8 +2161,14 @@
       <c r="K38" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
         <v>24</v>
       </c>
@@ -1976,8 +2202,14 @@
       <c r="K39" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
         <v>24</v>
       </c>
@@ -2011,8 +2243,14 @@
       <c r="K40" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L40" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
         <v>24</v>
       </c>
@@ -2046,8 +2284,14 @@
       <c r="K41" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>24</v>
       </c>
@@ -2081,8 +2325,14 @@
       <c r="K42" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>24</v>
       </c>
@@ -2116,8 +2366,14 @@
       <c r="K43" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L43" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
         <v>24</v>
       </c>
@@ -2151,8 +2407,14 @@
       <c r="K44" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L44" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
         <v>24</v>
       </c>
@@ -2186,8 +2448,14 @@
       <c r="K45" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L45" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
         <v>24</v>
       </c>
@@ -2221,8 +2489,14 @@
       <c r="K46" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L46" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
         <v>24</v>
       </c>
@@ -2256,8 +2530,14 @@
       <c r="K47" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L47" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
         <v>24</v>
       </c>
@@ -2291,8 +2571,14 @@
       <c r="K48" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L48" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
         <v>24</v>
       </c>
@@ -2326,8 +2612,14 @@
       <c r="K49" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L49" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
         <v>24</v>
       </c>
@@ -2361,8 +2653,14 @@
       <c r="K50" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L50" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>36</v>
       </c>
@@ -2396,8 +2694,14 @@
       <c r="K51" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L51" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
         <v>36</v>
       </c>
@@ -2431,8 +2735,14 @@
       <c r="K52" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L52" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
         <v>36</v>
       </c>
@@ -2466,8 +2776,14 @@
       <c r="K53" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L53" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
         <v>36</v>
       </c>
@@ -2501,8 +2817,14 @@
       <c r="K54" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L54" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="10" t="s">
         <v>36</v>
       </c>
@@ -2536,8 +2858,14 @@
       <c r="K55" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L55" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="10" t="s">
         <v>36</v>
       </c>
@@ -2571,8 +2899,14 @@
       <c r="K56" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L56" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
         <v>36</v>
       </c>
@@ -2606,8 +2940,14 @@
       <c r="K57" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L57" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="s">
         <v>36</v>
       </c>
@@ -2641,8 +2981,14 @@
       <c r="K58" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L58" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="s">
         <v>36</v>
       </c>
@@ -2676,8 +3022,14 @@
       <c r="K59" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L59" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
         <v>36</v>
       </c>
@@ -2711,8 +3063,14 @@
       <c r="K60" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L60" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
         <v>36</v>
       </c>
@@ -2746,8 +3104,14 @@
       <c r="K61" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L61" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
         <v>36</v>
       </c>
@@ -2781,8 +3145,14 @@
       <c r="K62" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L62" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
         <v>36</v>
       </c>
@@ -2816,8 +3186,14 @@
       <c r="K63" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L63" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="s">
         <v>36</v>
       </c>
@@ -2851,8 +3227,14 @@
       <c r="K64" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L64" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="10" t="s">
         <v>36</v>
       </c>
@@ -2886,8 +3268,14 @@
       <c r="K65" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L65" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="10" t="s">
         <v>36</v>
       </c>
@@ -2921,8 +3309,14 @@
       <c r="K66" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L66" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M66" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="10" t="s">
         <v>36</v>
       </c>
@@ -2956,8 +3350,14 @@
       <c r="K67" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L67" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M67" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="10" t="s">
         <v>36</v>
       </c>
@@ -2991,8 +3391,14 @@
       <c r="K68" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L68" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M68" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="10" t="s">
         <v>36</v>
       </c>
@@ -3026,8 +3432,14 @@
       <c r="K69" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L69" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M69" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="10" t="s">
         <v>36</v>
       </c>
@@ -3061,10 +3473,16 @@
       <c r="K70" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L70" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M70" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B71" s="1">
         <v>69</v>
@@ -3073,7 +3491,7 @@
         <v>41</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>3</v>
@@ -3096,10 +3514,16 @@
       <c r="K71" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L71" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M71" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B72" s="1">
         <v>70</v>
@@ -3108,7 +3532,7 @@
         <v>41</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>4</v>
@@ -3131,10 +3555,16 @@
       <c r="K72" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L72" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M72" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B73" s="1">
         <v>71</v>
@@ -3143,7 +3573,7 @@
         <v>41</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>5</v>
@@ -3166,10 +3596,16 @@
       <c r="K73" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L73" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M73" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B74" s="1">
         <v>72</v>
@@ -3178,7 +3614,7 @@
         <v>41</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>3</v>
@@ -3201,10 +3637,16 @@
       <c r="K74" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L74" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M74" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B75" s="1">
         <v>73</v>
@@ -3213,7 +3655,7 @@
         <v>41</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="E75" s="8" t="s">
         <v>4</v>
@@ -3236,10 +3678,16 @@
       <c r="K75" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L75" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M75" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B76" s="1">
         <v>74</v>
@@ -3248,7 +3696,7 @@
         <v>41</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>5</v>
@@ -3271,10 +3719,16 @@
       <c r="K76" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L76" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M76" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B77" s="1">
         <v>75</v>
@@ -3283,33 +3737,39 @@
         <v>25</v>
       </c>
       <c r="D77" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E77" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F77" s="8">
+        <v>0</v>
+      </c>
+      <c r="G77" s="8">
+        <v>0</v>
+      </c>
+      <c r="H77" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I77" s="8">
+        <v>0</v>
+      </c>
+      <c r="J77" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K77" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L77" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M77" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A78" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="E77" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F77" s="8">
-        <v>0</v>
-      </c>
-      <c r="G77" s="8">
-        <v>0</v>
-      </c>
-      <c r="H77" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I77" s="8">
-        <v>0</v>
-      </c>
-      <c r="J77" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K77" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A78" s="10" t="s">
-        <v>47</v>
       </c>
       <c r="B78" s="1">
         <v>76</v>
@@ -3318,10 +3778,10 @@
         <v>25</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F78" s="8">
         <v>0</v>
@@ -3341,10 +3801,16 @@
       <c r="K78" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L78" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M78" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B79" s="1">
         <v>77</v>
@@ -3353,10 +3819,10 @@
         <v>25</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F79" s="8">
         <v>0</v>
@@ -3376,10 +3842,16 @@
       <c r="K79" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L79" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M79" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B80" s="1">
         <v>78</v>
@@ -3388,10 +3860,10 @@
         <v>25</v>
       </c>
       <c r="D80" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E80" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="E80" s="8" t="s">
-        <v>46</v>
       </c>
       <c r="F80" s="8" t="s">
         <v>15</v>
@@ -3411,10 +3883,16 @@
       <c r="K80" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L80" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M80" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B81" s="1">
         <v>79</v>
@@ -3423,10 +3901,10 @@
         <v>25</v>
       </c>
       <c r="D81" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E81" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="E81" s="8" t="s">
-        <v>46</v>
       </c>
       <c r="F81" s="8" t="s">
         <v>16</v>
@@ -3446,10 +3924,16 @@
       <c r="K81" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L81" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M81" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B82" s="1">
         <v>80</v>
@@ -3458,7 +3942,7 @@
         <v>31</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="E82" s="8" t="s">
         <v>3</v>
@@ -3481,10 +3965,16 @@
       <c r="K82" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L82" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M82" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B83" s="1">
         <v>81</v>
@@ -3493,7 +3983,7 @@
         <v>31</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>4</v>
@@ -3516,10 +4006,16 @@
       <c r="K83" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L83" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M83" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B84" s="1">
         <v>82</v>
@@ -3528,7 +4024,7 @@
         <v>31</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>5</v>
@@ -3551,10 +4047,16 @@
       <c r="K84" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L84" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M84" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B85" s="1">
         <v>83</v>
@@ -3563,7 +4065,7 @@
         <v>31</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>3</v>
@@ -3584,12 +4086,18 @@
         <v>14</v>
       </c>
       <c r="K85" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="L85" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M85" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B86" s="1">
         <v>84</v>
@@ -3598,7 +4106,7 @@
         <v>31</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>4</v>
@@ -3619,12 +4127,18 @@
         <v>14</v>
       </c>
       <c r="K86" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="L86" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M86" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B87" s="1">
         <v>85</v>
@@ -3633,7 +4147,7 @@
         <v>31</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>5</v>
@@ -3654,12 +4168,18 @@
         <v>14</v>
       </c>
       <c r="K87" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="L87" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M87" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B88" s="1">
         <v>86</v>
@@ -3668,7 +4188,7 @@
         <v>30</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>3</v>
@@ -3689,12 +4209,18 @@
         <v>14</v>
       </c>
       <c r="K88" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="L88" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M88" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B89" s="1">
         <v>87</v>
@@ -3703,7 +4229,7 @@
         <v>30</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>4</v>
@@ -3724,12 +4250,18 @@
         <v>14</v>
       </c>
       <c r="K89" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="L89" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M89" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B90" s="1">
         <v>88</v>
@@ -3738,7 +4270,7 @@
         <v>30</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>5</v>
@@ -3759,12 +4291,18 @@
         <v>14</v>
       </c>
       <c r="K90" s="9" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+      <c r="L90" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M90" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B1:M1"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>